<commit_message>
ECP-1149: implements amend budget
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/test/java/org/estatio/module/capex/integtests/project/BudgetITPR001.xlsx
+++ b/estatioapp/app/src/test/java/org/estatio/module/capex/integtests/project/BudgetITPR001.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/test/java/org/estatio/module/capex/integtests/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDAC107-D84D-8D49-A37B-56954F88E527}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0928040-404E-684C-B697-32D935ABB343}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Project Reference</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>ITWT005</t>
+  </si>
+  <si>
+    <t>Budget Version</t>
   </si>
 </sst>
 </file>
@@ -392,11 +395,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -406,7 +409,7 @@
     <col min="3" max="3" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,28 +417,37 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
         <v>123456.78</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
         <v>9876543.2100000009</v>
       </c>
     </row>

</xml_diff>